<commit_message>
exporting 1 month's orders
changed the order query on the exporter
</commit_message>
<xml_diff>
--- a/storage/exports/JagerLabels_2017-11-14-2017-12-14.xlsx
+++ b/storage/exports/JagerLabels_2017-11-14-2017-12-14.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>orderid</t>
   </si>
@@ -48,7 +48,7 @@
     <t>Scott Brown (TEST)</t>
   </si>
   <si>
-    <t>2017-12-14 11:27:19</t>
+    <t>2017-11-14 11:27:19</t>
   </si>
   <si>
     <t>2.00</t>
@@ -57,64 +57,7 @@
     <t>Jägermeister 2cl Bottle Label (Applied to Bottles)</t>
   </si>
   <si>
-    <t>JGkMPdxwsS</t>
-  </si>
-  <si>
-    <t>2017-12-14 11:33:22</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>2.50</t>
-  </si>
-  <si>
-    <t>Jägermeister 70cl Bottle Label (Label Only)</t>
-  </si>
-  <si>
-    <t>JG4hxRfY0S</t>
-  </si>
-  <si>
-    <t>2017-12-14 12:48:48</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>50.00</t>
-  </si>
-  <si>
-    <t>JGBXsj3FrB</t>
-  </si>
-  <si>
-    <t>2017-12-14 12:49:43</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>10.00</t>
-  </si>
-  <si>
-    <t>Jägermeister 2cl Bottle Label (Label Only)</t>
-  </si>
-  <si>
     <t>items</t>
-  </si>
-  <si>
-    <t>12.00</t>
-  </si>
-  <si>
-    <t>Jägermeister 2cl Bottle Label (Applied to Bottles), Jägermeister 2cl Bottle Label (Label Only)</t>
-  </si>
-  <si>
-    <t>JGcGbB2i3N</t>
-  </si>
-  <si>
-    <t>2017-12-14 15:19:39</t>
-  </si>
-  <si>
-    <t>0.00</t>
   </si>
 </sst>
 </file>
@@ -454,7 +397,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,98 +458,6 @@
       </c>
       <c r="G2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -644,7 +495,7 @@
     <col min="3" max="3" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="23.422852" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="111.972656" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="60.128174" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -664,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -685,83 +536,6 @@
       </c>
       <c r="F2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>